<commit_message>
migrating date storage format from number to ISO string
</commit_message>
<xml_diff>
--- a/Dummy Data Generator.xlsx
+++ b/Dummy Data Generator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ignindra\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Indra\Sandbox\Mitrais-Training-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="165">
   <si>
     <t>lastname</t>
   </si>
@@ -294,6 +294,231 @@
   </si>
   <si>
     <t>ph.jpg</t>
+  </si>
+  <si>
+    <t>1953-06-16T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1954-10-20T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1955-02-22T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1958-08-13T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1960-06-14T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1963-09-05T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1963-11-15T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1975-07-31T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1977-02-11T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1978-01-17T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1979-06-26T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1988-09-30T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1990-12-07T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1991-08-20T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1994-08-05T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1995-04-07T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1996-07-16T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2000-08-30T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2000-12-01T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2002-10-18T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2003-06-18T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2005-04-19T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2008-09-05T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2010-12-01T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2017-08-21T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1962-01-25T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1968-12-13T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1972-07-05T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1976-07-26T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1977-05-03T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1978-09-20T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1979-01-30T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1985-05-20T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1985-10-07T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1985-11-13T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1989-06-21T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1989-08-14T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1990-01-02T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1990-10-31T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1990-12-26T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1991-07-17T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1998-05-12T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1998-07-03T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2001-01-03T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2002-03-26T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2004-02-23T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2004-05-14T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2006-01-30T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2009-04-22T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2010-09-22T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1957-01-10T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1961-08-07T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1965-03-30T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1967-05-09T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1968-05-15T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1974-12-26T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1975-09-12T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1976-11-23T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1977-04-01T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1979-07-17T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1981-10-12T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1985-01-04T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1985-09-04T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1986-05-19T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1987-10-29T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1988-02-25T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1988-12-15T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1997-10-29T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>1998-12-10T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2000-11-06T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2006-08-01T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2006-09-28T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2007-02-21T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2012-03-19T17:00:00.000Z</t>
+  </si>
+  <si>
+    <t>2013-09-20T17:00:00.000Z</t>
   </si>
 </sst>
 </file>
@@ -614,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,9 +914,8 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <f t="shared" ref="A2:P17" ca="1" si="0">RANDBETWEEN(61200000, 1493139600000)</f>
-        <v>292499549220</v>
+      <c r="A2" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Division 1","Division 2","Division 3","Division 4","Division 5")</f>
@@ -699,7 +923,7 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">CONCATENATE("user", RANDBETWEEN(1,100), "@mail.com")</f>
-        <v>user99@mail.com</v>
+        <v>user26@mail.com</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -710,11 +934,10 @@
       </c>
       <c r="F2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,6),"SE - JP","SE - PG","SE - AP","SE - AN","SQ - JT","SQ - TS")</f>
-        <v>SQ - JT</v>
-      </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G26" ca="1" si="1">RANDBETWEEN(61200000, 1493139600000)</f>
-        <v>1210840165891</v>
+        <v>SE - AP</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>89</v>
@@ -722,61 +945,58 @@
       <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,4),"Bali","Jakarta","Bandung","Yogyakarta")</f>
-        <v>Bali</v>
+      <c r="J2">
+        <f ca="1">RANDBETWEEN(1,4)</f>
+        <v>3</v>
       </c>
       <c r="K2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,5),"Single","Married", "Divorced","Widow/Widower", "Other")</f>
-        <v>Divorced</v>
+        <v>Married</v>
       </c>
       <c r="L2" t="s">
         <v>64</v>
       </c>
       <c r="M2" s="1">
         <f ca="1">RANDBETWEEN(628111111111, 700000000000)</f>
-        <v>670011724759</v>
+        <v>651200074163</v>
       </c>
       <c r="N2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Contract","Permanent")</f>
-        <v>Permanent</v>
+        <v>Contract</v>
       </c>
       <c r="O2" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,10),"Sub Division 1","Sub Division 2","Sub Division 3","Sub Division 4","Sub Division 5","Sub Division 6","Sub Division 7","Sub Division 8","Sub Division 9","Sub Division 10")</f>
-        <v>Sub Division 9</v>
-      </c>
-      <c r="P2" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>986989361882</v>
+        <v>Sub Division 2</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1142411101415</v>
+      <c r="A3" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B26" ca="1" si="2">CHOOSE(RANDBETWEEN(1,5),"Division 1","Division 2","Division 3","Division 4","Division 5")</f>
-        <v>Division 5</v>
+        <f t="shared" ref="B3:B26" ca="1" si="0">CHOOSE(RANDBETWEEN(1,5),"Division 1","Division 2","Division 3","Division 4","Division 5")</f>
+        <v>Division 1</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C26" ca="1" si="3">CONCATENATE("user", RANDBETWEEN(1,100), "@mail.com")</f>
-        <v>user20@mail.com</v>
+        <f t="shared" ref="C3:C26" ca="1" si="1">CONCATENATE("user", RANDBETWEEN(1,100), "@mail.com")</f>
+        <v>user44@mail.com</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E26" ca="1" si="4">CHOOSE(RANDBETWEEN(1,3),"Male","Female","Other")</f>
-        <v>Other</v>
+        <f t="shared" ref="E3:E26" ca="1" si="2">CHOOSE(RANDBETWEEN(1,3),"Male","Female","Other")</f>
+        <v>Female</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F26" ca="1" si="5">CHOOSE(RANDBETWEEN(1,6),"SE - JP","SE - PG","SE - AP","SE - AN","SQ - JT","SQ - TS")</f>
-        <v>SQ - TS</v>
-      </c>
-      <c r="G3" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1079874231776</v>
+        <f t="shared" ref="F3:F26" ca="1" si="3">CHOOSE(RANDBETWEEN(1,6),"SE - JP","SE - PG","SE - AP","SE - AN","SQ - JT","SQ - TS")</f>
+        <v>SQ - JT</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>89</v>
@@ -784,61 +1004,58 @@
       <c r="I3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J26" ca="1" si="6">CHOOSE(RANDBETWEEN(1,4),"Bali","Jakarta","Bandung","Yogyakarta")</f>
-        <v>Jakarta</v>
+      <c r="J3">
+        <f t="shared" ref="J3:J26" ca="1" si="4">RANDBETWEEN(1,4)</f>
+        <v>4</v>
       </c>
       <c r="K3" t="str">
-        <f t="shared" ref="K3:K26" ca="1" si="7">CHOOSE(RANDBETWEEN(1,5),"Single","Married", "Divorced","Widow/Widower", "Other")</f>
-        <v>Other</v>
+        <f t="shared" ref="K3:K26" ca="1" si="5">CHOOSE(RANDBETWEEN(1,5),"Single","Married", "Divorced","Widow/Widower", "Other")</f>
+        <v>Single</v>
       </c>
       <c r="L3" t="s">
         <v>65</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" ref="M3:M26" ca="1" si="8">RANDBETWEEN(628111111111, 700000000000)</f>
-        <v>677573687403</v>
+        <f t="shared" ref="M3:M26" ca="1" si="6">RANDBETWEEN(628111111111, 700000000000)</f>
+        <v>692520247951</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N26" ca="1" si="9">CHOOSE(RANDBETWEEN(1,2),"Contract","Permanent")</f>
-        <v>Contract</v>
+        <f t="shared" ref="N3:N26" ca="1" si="7">CHOOSE(RANDBETWEEN(1,2),"Contract","Permanent")</f>
+        <v>Permanent</v>
       </c>
       <c r="O3" t="str">
-        <f t="shared" ref="O3:O26" ca="1" si="10">CHOOSE(RANDBETWEEN(1,10),"Sub Division 1","Sub Division 2","Sub Division 3","Sub Division 4","Sub Division 5","Sub Division 6","Sub Division 7","Sub Division 8","Sub Division 9","Sub Division 10")</f>
-        <v>Sub Division 8</v>
-      </c>
-      <c r="P3" s="1">
+        <f t="shared" ref="O3:O26" ca="1" si="8">CHOOSE(RANDBETWEEN(1,10),"Sub Division 1","Sub Division 2","Sub Division 3","Sub Division 4","Sub Division 5","Sub Division 6","Sub Division 7","Sub Division 8","Sub Division 9","Sub Division 10")</f>
+        <v>Sub Division 4</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>293453208431</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>608830254082</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 2</v>
+        <v>Division 3</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user34@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user67@mail.com</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
       <c r="E4" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Male</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SQ - TS</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>696266214098</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - JP</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>89</v>
@@ -846,61 +1063,58 @@
       <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bali</v>
+      <c r="J4">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
       </c>
       <c r="K4" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Widow/Widower</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Married</v>
       </c>
       <c r="L4" t="s">
         <v>66</v>
       </c>
       <c r="M4" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>688333732262</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O4" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>655819584403</v>
-      </c>
-      <c r="N4" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O4" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 8</v>
-      </c>
-      <c r="P4" s="1">
+        <v>Sub Division 2</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>840940173492</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>83624164311</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 5</v>
+        <v>Division 2</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user68@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user54@mail.com</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Male</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Female</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - PG</v>
-      </c>
-      <c r="G5" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>202029839451</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SQ - TS</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>89</v>
@@ -908,61 +1122,58 @@
       <c r="I5" t="s">
         <v>22</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Jakarta</v>
+      <c r="J5">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Widow/Widower</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Single</v>
       </c>
       <c r="L5" t="s">
         <v>67</v>
       </c>
       <c r="M5" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>687615904756</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O5" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>636840715001</v>
-      </c>
-      <c r="N5" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 7</v>
-      </c>
-      <c r="P5" s="1">
+        <v>Sub Division 10</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>1245025395118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>317874522848</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" ca="1" si="2"/>
         <v>Division 3</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user17@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user100@mail.com</v>
       </c>
       <c r="D6" t="s">
         <v>23</v>
       </c>
       <c r="E6" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Male</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Female</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - AN</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>550194021802</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - PG</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>89</v>
@@ -970,61 +1181,58 @@
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bandung</v>
+      <c r="J6">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Other</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Single</v>
       </c>
       <c r="L6" t="s">
         <v>68</v>
       </c>
       <c r="M6" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>645559801386</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O6" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>689637158920</v>
-      </c>
-      <c r="N6" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 3</v>
-      </c>
-      <c r="P6" s="1">
+        <v>Sub Division 1</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>94647669305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>856211583412</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 3</v>
+        <v>Division 1</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user88@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user80@mail.com</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
       </c>
       <c r="E7" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Other</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Male</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SQ - JT</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>744334986331</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - PG</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>89</v>
@@ -1032,61 +1240,58 @@
       <c r="I7" t="s">
         <v>26</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bandung</v>
+      <c r="J7">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
       </c>
       <c r="K7" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Single</v>
       </c>
       <c r="L7" t="s">
         <v>69</v>
       </c>
       <c r="M7" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>640183751935</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O7" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>696726813998</v>
-      </c>
-      <c r="N7" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 2</v>
-      </c>
-      <c r="P7" s="1">
+        <v>Sub Division 10</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>51315722764</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>762495221464</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 5</v>
+        <v>Division 4</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user77@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user92@mail.com</v>
       </c>
       <c r="D8" t="s">
         <v>27</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Female</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Other</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - PG</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>418540729477</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - AN</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>89</v>
@@ -1094,61 +1299,58 @@
       <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="J8" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Yogyakarta</v>
+      <c r="J8">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Divorced</v>
       </c>
       <c r="L8" t="s">
         <v>70</v>
       </c>
       <c r="M8" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>677586851123</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O8" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>677265360907</v>
-      </c>
-      <c r="N8" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 10</v>
-      </c>
-      <c r="P8" s="1">
+        <v>Sub Division 8</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>554185822447</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>653997269212</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 5</v>
+        <v>Division 2</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user38@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user24@mail.com</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Female</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Male</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SQ - JT</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>692895968155</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - AN</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>89</v>
@@ -1156,61 +1358,58 @@
       <c r="I9" t="s">
         <v>30</v>
       </c>
-      <c r="J9" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bali</v>
+      <c r="J9">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Married</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Single</v>
       </c>
       <c r="L9" t="s">
         <v>71</v>
       </c>
       <c r="M9" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>657097567345</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O9" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>682165792385</v>
-      </c>
-      <c r="N9" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 7</v>
-      </c>
-      <c r="P9" s="1">
+        <v>Sub Division 9</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>259631790596</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>955266933378</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" ca="1" si="2"/>
         <v>Division 4</v>
       </c>
       <c r="C10" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user44@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user80@mail.com</v>
       </c>
       <c r="D10" t="s">
         <v>31</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Other</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Female</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SQ - TS</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>700006306187</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - AN</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>123</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>89</v>
@@ -1218,61 +1417,58 @@
       <c r="I10" t="s">
         <v>32</v>
       </c>
-      <c r="J10" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Jakarta</v>
+      <c r="J10">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Single</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Married</v>
       </c>
       <c r="L10" t="s">
         <v>72</v>
       </c>
       <c r="M10" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>689834703595</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O10" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>634453855533</v>
-      </c>
-      <c r="N10" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 6</v>
-      </c>
-      <c r="P10" s="1">
+        <v>Sub Division 1</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>813919830552</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1375331580762</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 2</v>
+        <v>Division 1</v>
       </c>
       <c r="C11" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user81@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user73@mail.com</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Female</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Other</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" ca="1" si="3"/>
         <v>SE - JP</v>
       </c>
-      <c r="G11" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1317063773737</v>
+      <c r="G11" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>89</v>
@@ -1280,61 +1476,58 @@
       <c r="I11" t="s">
         <v>34</v>
       </c>
-      <c r="J11" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bali</v>
+      <c r="J11">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
       </c>
       <c r="K11" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Single</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Widow/Widower</v>
       </c>
       <c r="L11" t="s">
         <v>73</v>
       </c>
       <c r="M11" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>652959775910</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O11" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>666613580852</v>
-      </c>
-      <c r="N11" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 1</v>
-      </c>
-      <c r="P11" s="1">
+        <v>Sub Division 4</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>20426033633</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>1115098519991</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" ca="1" si="2"/>
         <v>Division 1</v>
       </c>
       <c r="C12" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user60@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user16@mail.com</v>
       </c>
       <c r="D12" t="s">
         <v>35</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Male</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Female</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - PG</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1055566321120</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - JP</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>89</v>
@@ -1342,61 +1535,58 @@
       <c r="I12" t="s">
         <v>36</v>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bandung</v>
+      <c r="J12">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="K12" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Divorced</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Married</v>
       </c>
       <c r="L12" t="s">
         <v>74</v>
       </c>
       <c r="M12" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>644379986257</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>634704293900</v>
-      </c>
-      <c r="N12" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 4</v>
-      </c>
-      <c r="P12" s="1">
+        <v>Sub Division 10</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>813023787273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>769306756017</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" ca="1" si="2"/>
         <v>Division 4</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user70@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user97@mail.com</v>
       </c>
       <c r="D13" t="s">
         <v>37</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Male</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Other</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - AN</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>573914966280</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - JP</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>89</v>
@@ -1404,61 +1594,58 @@
       <c r="I13" t="s">
         <v>38</v>
       </c>
-      <c r="J13" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Yogyakarta</v>
+      <c r="J13">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Single</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Other</v>
       </c>
       <c r="L13" t="s">
         <v>69</v>
       </c>
       <c r="M13" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>696454030204</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>692832034583</v>
-      </c>
-      <c r="N13" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 2</v>
-      </c>
-      <c r="P13" s="1">
+        <v>Sub Division 1</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>1341556886586</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>3845827012</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 5</v>
+        <v>Division 3</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user48@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user34@mail.com</v>
       </c>
       <c r="D14" t="s">
         <v>39</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Other</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - JP</v>
-      </c>
-      <c r="G14" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>41115751321</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SQ - JT</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>127</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>89</v>
@@ -1466,61 +1653,58 @@
       <c r="I14" t="s">
         <v>40</v>
       </c>
-      <c r="J14" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bali</v>
+      <c r="J14">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Other</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Single</v>
       </c>
       <c r="L14" t="s">
         <v>75</v>
       </c>
       <c r="M14" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>692750143359</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>631249542589</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 2</v>
-      </c>
-      <c r="P14" s="1">
+        <v>Sub Division 8</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>41050665114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>194661809105</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 1</v>
+        <v>Division 4</v>
       </c>
       <c r="C15" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user86@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user27@mail.com</v>
       </c>
       <c r="D15" t="s">
         <v>41</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Other</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Female</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SQ - TS</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>650990346013</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - PG</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>89</v>
@@ -1528,61 +1712,58 @@
       <c r="I15" t="s">
         <v>42</v>
       </c>
-      <c r="J15" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Jakarta</v>
+      <c r="J15">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
       <c r="K15" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Married</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Widow/Widower</v>
       </c>
       <c r="L15" t="s">
         <v>76</v>
       </c>
       <c r="M15" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>690254950992</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>664217432141</v>
-      </c>
-      <c r="N15" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 6</v>
-      </c>
-      <c r="P15" s="1">
+        <v>Sub Division 8</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>1470717243369</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>270346562123</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 3</v>
+        <v>Division 4</v>
       </c>
       <c r="C16" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user15@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user37@mail.com</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Other</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Male</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - AP</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>684187872816</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - JP</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>89</v>
@@ -1590,61 +1771,58 @@
       <c r="I16" t="s">
         <v>44</v>
       </c>
-      <c r="J16" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bandung</v>
+      <c r="J16">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Married</v>
       </c>
       <c r="L16" t="s">
         <v>77</v>
       </c>
       <c r="M16" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>659515779762</v>
+      </c>
+      <c r="N16" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>661120826053</v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 1</v>
-      </c>
-      <c r="P16" s="1">
+        <v>Sub Division 10</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>401099803003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>252364265632</v>
-      </c>
-      <c r="B17" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 1</v>
+        <v>Division 5</v>
       </c>
       <c r="C17" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user20@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user87@mail.com</v>
       </c>
       <c r="D17" t="s">
         <v>45</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Female</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - PG</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>726504889892</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - AN</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>89</v>
@@ -1652,61 +1830,58 @@
       <c r="I17" t="s">
         <v>46</v>
       </c>
-      <c r="J17" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Yogyakarta</v>
+      <c r="J17">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
       </c>
       <c r="K17" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Divorced</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Widow/Widower</v>
       </c>
       <c r="L17" t="s">
         <v>78</v>
       </c>
       <c r="M17" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>635800951635</v>
+      </c>
+      <c r="N17" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>691786283692</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 5</v>
-      </c>
-      <c r="P17" s="1">
+        <v>Sub Division 9</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>900180822317</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <f t="shared" ref="A18:P26" ca="1" si="11">RANDBETWEEN(61200000, 1493139600000)</f>
-        <v>785067426039</v>
-      </c>
-      <c r="B18" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 3</v>
+        <v>Division 2</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user2@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user83@mail.com</v>
       </c>
       <c r="D18" t="s">
         <v>47</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Male</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Other</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - AN</v>
-      </c>
-      <c r="G18" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1376799347788</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - PG</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>131</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>89</v>
@@ -1714,61 +1889,58 @@
       <c r="I18" t="s">
         <v>48</v>
       </c>
-      <c r="J18" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bali</v>
+      <c r="J18">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="K18" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Single</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Other</v>
       </c>
       <c r="L18" t="s">
         <v>79</v>
       </c>
       <c r="M18" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>647190136515</v>
+      </c>
+      <c r="N18" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>654188852292</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 9</v>
-      </c>
-      <c r="P18" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>1130693171756</v>
+        <v>Sub Division 6</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>212869726308</v>
+      <c r="A19" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Division 2</v>
       </c>
       <c r="C19" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user61@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user11@mail.com</v>
       </c>
       <c r="D19" t="s">
         <v>49</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Male</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - AP</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>257513931452</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SQ - JT</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>132</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>89</v>
@@ -1776,61 +1948,58 @@
       <c r="I19" t="s">
         <v>50</v>
       </c>
-      <c r="J19" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Yogyakarta</v>
+      <c r="J19">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Single</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Widow/Widower</v>
       </c>
       <c r="L19" t="s">
         <v>80</v>
       </c>
       <c r="M19" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>645502070253</v>
+      </c>
+      <c r="N19" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>671234329835</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O19" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 4</v>
-      </c>
-      <c r="P19" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>1058239289492</v>
+        <v>Sub Division 1</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>4759478681</v>
+      <c r="A20" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Division 2</v>
       </c>
       <c r="C20" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user38@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user29@mail.com</v>
       </c>
       <c r="D20" t="s">
         <v>32</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Male</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Other</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SQ - JT</v>
-      </c>
-      <c r="G20" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1112287594919</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - AN</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>133</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>89</v>
@@ -1838,61 +2007,58 @@
       <c r="I20" t="s">
         <v>51</v>
       </c>
-      <c r="J20" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bali</v>
+      <c r="J20">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Married</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Divorced</v>
       </c>
       <c r="L20" t="s">
         <v>81</v>
       </c>
       <c r="M20" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>649040197795</v>
+      </c>
+      <c r="N20" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O20" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>642660126643</v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O20" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 1</v>
-      </c>
-      <c r="P20" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>1284862346208</v>
+        <v>Sub Division 8</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>489283686124</v>
+      <c r="A21" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Division 3</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user94@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user57@mail.com</v>
       </c>
       <c r="D21" t="s">
         <v>52</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Male</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Other</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - PG</v>
-      </c>
-      <c r="G21" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>494883075526</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - JP</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>89</v>
@@ -1900,61 +2066,58 @@
       <c r="I21" t="s">
         <v>53</v>
       </c>
-      <c r="J21" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bandung</v>
+      <c r="J21">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Other</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Widow/Widower</v>
       </c>
       <c r="L21" t="s">
         <v>82</v>
       </c>
       <c r="M21" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>690617030401</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O21" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>699835885044</v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 5</v>
-      </c>
-      <c r="P21" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>1236631551902</v>
+        <v>Sub Division 3</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>1132190239400</v>
+      <c r="A22" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Division 5</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user4@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user57@mail.com</v>
       </c>
       <c r="D22" t="s">
         <v>54</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Male</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - AN</v>
-      </c>
-      <c r="G22" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1058069769431</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - PG</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>89</v>
@@ -1962,61 +2125,58 @@
       <c r="I22" t="s">
         <v>55</v>
       </c>
-      <c r="J22" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Jakarta</v>
+      <c r="J22">
+        <f t="shared" ca="1" si="4"/>
+        <v>1</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Single</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Married</v>
       </c>
       <c r="L22" t="s">
         <v>83</v>
       </c>
       <c r="M22" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>691191841910</v>
+      </c>
+      <c r="N22" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O22" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>635857819173</v>
-      </c>
-      <c r="N22" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O22" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 7</v>
-      </c>
-      <c r="P22" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>639477416334</v>
+        <v>Sub Division 10</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>1400744482338</v>
+      <c r="A23" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Division 1</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user45@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user85@mail.com</v>
       </c>
       <c r="D23" t="s">
         <v>56</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Male</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - AP</v>
-      </c>
-      <c r="G23" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1279572920401</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - JP</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>89</v>
@@ -2024,61 +2184,58 @@
       <c r="I23" t="s">
         <v>57</v>
       </c>
-      <c r="J23" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bandung</v>
+      <c r="J23">
+        <f t="shared" ca="1" si="4"/>
+        <v>2</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="5"/>
         <v>Married</v>
       </c>
       <c r="L23" t="s">
         <v>84</v>
       </c>
       <c r="M23" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>654910696945</v>
+      </c>
+      <c r="N23" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O23" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>662885951680</v>
-      </c>
-      <c r="N23" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Permanent</v>
-      </c>
-      <c r="O23" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 8</v>
-      </c>
-      <c r="P23" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>477292573410</v>
+        <v>Sub Division 5</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>227225093447</v>
+      <c r="A24" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Division 2</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user65@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user88@mail.com</v>
       </c>
       <c r="D24" t="s">
         <v>58</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="2"/>
         <v>Other</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SE - JP</v>
-      </c>
-      <c r="G24" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>284454564868</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SQ - JT</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>137</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>89</v>
@@ -2086,61 +2243,58 @@
       <c r="I24" t="s">
         <v>59</v>
       </c>
-      <c r="J24" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Yogyakarta</v>
+      <c r="J24">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Widow/Widower</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Divorced</v>
       </c>
       <c r="L24" t="s">
         <v>85</v>
       </c>
       <c r="M24" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>673720709888</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O24" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>636201464153</v>
-      </c>
-      <c r="N24" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O24" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 5</v>
-      </c>
-      <c r="P24" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>698490694687</v>
+        <v>Sub Division 8</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>1350286417573</v>
+      <c r="A25" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Division 3</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user13@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user14@mail.com</v>
       </c>
       <c r="D25" t="s">
         <v>60</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Other</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Male</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SQ - JT</v>
-      </c>
-      <c r="G25" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>1340701578265</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SE - AP</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>89</v>
@@ -2148,61 +2302,58 @@
       <c r="I25" t="s">
         <v>61</v>
       </c>
-      <c r="J25" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bali</v>
+      <c r="J25">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Single</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Widow/Widower</v>
       </c>
       <c r="L25" t="s">
         <v>86</v>
       </c>
       <c r="M25" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>680287110954</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Permanent</v>
+      </c>
+      <c r="O25" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>694212371429</v>
-      </c>
-      <c r="N25" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O25" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 3</v>
-      </c>
-      <c r="P25" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>850932979803</v>
+        <v>Sub Division 9</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>405468667109</v>
+      <c r="A26" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Division 5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>Division 4</v>
       </c>
       <c r="C26" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>user41@mail.com</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>user35@mail.com</v>
       </c>
       <c r="D26" t="s">
         <v>62</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>Female</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>Male</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" ca="1" si="5"/>
-        <v>SQ - JT</v>
-      </c>
-      <c r="G26" s="1">
-        <f t="shared" ca="1" si="1"/>
-        <v>430830804064</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>SQ - TS</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>139</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>89</v>
@@ -2210,32 +2361,31 @@
       <c r="I26" t="s">
         <v>63</v>
       </c>
-      <c r="J26" t="str">
-        <f t="shared" ca="1" si="6"/>
-        <v>Bali</v>
+      <c r="J26">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
       </c>
       <c r="K26" t="str">
-        <f t="shared" ca="1" si="7"/>
-        <v>Widow/Widower</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>Married</v>
       </c>
       <c r="L26" t="s">
         <v>87</v>
       </c>
       <c r="M26" s="1">
+        <f t="shared" ca="1" si="6"/>
+        <v>656856531555</v>
+      </c>
+      <c r="N26" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>Contract</v>
+      </c>
+      <c r="O26" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>691975873945</v>
-      </c>
-      <c r="N26" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v>Contract</v>
-      </c>
-      <c r="O26" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>Sub Division 6</v>
-      </c>
-      <c r="P26" s="1">
-        <f t="shared" ca="1" si="11"/>
-        <v>1313311651494</v>
+        <v>Sub Division 1</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>